<commit_message>
user names on excel db and info box
</commit_message>
<xml_diff>
--- a/sources/EDT-Barbosa-lucaspradodeoliveira.xlsx
+++ b/sources/EDT-Barbosa-lucaspradodeoliveira.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="3" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME_MENSAL" sheetId="1" state="visible" r:id="rId1"/>
@@ -31713,9 +31713,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:L30"/>
+  <dimension ref="B2:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -32736,10 +32736,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>1002/2501/2502</t>
-        </is>
+      <c r="B24" t="n">
+        <v>2802</v>
       </c>
       <c r="C24">
         <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B24,Recebíveis!N:N,"Futuro")</f>
@@ -32784,7 +32782,7 @@
     </row>
     <row r="25">
       <c r="B25" t="n">
-        <v>2802</v>
+        <v>501</v>
       </c>
       <c r="C25">
         <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B25,Recebíveis!N:N,"Futuro")</f>
@@ -32829,7 +32827,7 @@
     </row>
     <row r="26">
       <c r="B26" t="n">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C26">
         <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B26,Recebíveis!N:N,"Futuro")</f>
@@ -32874,7 +32872,7 @@
     </row>
     <row r="27">
       <c r="B27" t="n">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C27">
         <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B27,Recebíveis!N:N,"Futuro")</f>
@@ -32919,7 +32917,7 @@
     </row>
     <row r="28">
       <c r="B28" t="n">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C28">
         <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B28,Recebíveis!N:N,"Futuro")</f>
@@ -32964,7 +32962,7 @@
     </row>
     <row r="29">
       <c r="B29" t="n">
-        <v>505</v>
+        <v>2302</v>
       </c>
       <c r="C29">
         <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B29,Recebíveis!N:N,"Futuro")</f>
@@ -33004,51 +33002,6 @@
       </c>
       <c r="L29">
         <f>IF(K29&lt;=30,INFORME_MENSAL!$A$3,IF(K29&lt;=60,INFORME_MENSAL!$A$4,IF(K29&lt;=90,INFORME_MENSAL!$A$5,IF(K29&lt;=120,INFORME_MENSAL!$A$6,IF(K29&lt;=150,INFORME_MENSAL!$A$7,IF(K29&lt;=180,INFORME_MENSAL!$A$8,IF(K29&lt;=360,INFORME_MENSAL!$A$9,IF(K29&gt;360,INFORME_MENSAL!$A$10))))))))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="n">
-        <v>2302</v>
-      </c>
-      <c r="C30">
-        <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B30,Recebíveis!N:N,"Futuro")</f>
-        <v/>
-      </c>
-      <c r="D30">
-        <f>SUMIFS(Recebíveis!L:L,Recebíveis!A:A,'Base Contratos'!B30,Recebíveis!N:N,"Atraso")</f>
-        <v/>
-      </c>
-      <c r="E30">
-        <f>SUMIFS(Recebíveis!P:P,Recebíveis!A:A,'Base Contratos'!B30)</f>
-        <v/>
-      </c>
-      <c r="F30">
-        <f>_xlfn.MAXIFS(Recebíveis!Q:Q,Recebíveis!A:A,'Base Contratos'!B30)</f>
-        <v/>
-      </c>
-      <c r="G30">
-        <f>IF(F30=0,"Em dia",IF(F30&lt;=15,"Até 15",IF(F30&lt;=30,"Entre 15 e 30",IF(F30&lt;=60,"Entre 30 e 60",IF(F30&lt;=90,"Entre 60 e 90",IF(F30&lt;=120,"Entre 90 e 120",IF(F30&lt;=150,"Entre 120 e 150",IF(F30&lt;=180,"Entre 150 e 180","Superior a 180"))))))))</f>
-        <v/>
-      </c>
-      <c r="H30">
-        <f>_xlfn.XLOOKUP(B30,'Relação de Contratos'!A:A,'Relação de Contratos'!G:G)</f>
-        <v/>
-      </c>
-      <c r="I30">
-        <f>IFERROR(E30/H30,"")</f>
-        <v/>
-      </c>
-      <c r="J30">
-        <f>_xlfn.MAXIFS(Recebíveis!G:G,Recebíveis!A:A,'Base Contratos'!B30)</f>
-        <v/>
-      </c>
-      <c r="K30">
-        <f>J30-'Relatório Consolidado'!$J$4</f>
-        <v/>
-      </c>
-      <c r="L30">
-        <f>IF(K30&lt;=30,INFORME_MENSAL!$A$3,IF(K30&lt;=60,INFORME_MENSAL!$A$4,IF(K30&lt;=90,INFORME_MENSAL!$A$5,IF(K30&lt;=120,INFORME_MENSAL!$A$6,IF(K30&lt;=150,INFORME_MENSAL!$A$7,IF(K30&lt;=180,INFORME_MENSAL!$A$8,IF(K30&lt;=360,INFORME_MENSAL!$A$9,IF(K30&gt;360,INFORME_MENSAL!$A$10))))))))</f>
         <v/>
       </c>
     </row>
@@ -33067,7 +33020,7 @@
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
@@ -33321,7 +33274,7 @@
         <v/>
       </c>
       <c r="Z2">
-        <f>IF(X2="Antecipação",IF(W2&lt;=30,INFORME_MENSAL!$A$21,IF(W2&lt;=60,INFORME_MENSAL!$A$22,IF(W2&lt;=90,INFORME_MENSAL!$A$23,IF(W2&lt;=120,INFORME_MENSAL!$A$24,IF(W2&lt;=150,INFORME_MENSAL!$A$25,IF(W2&lt;=180,INFORME_MENSAL!$A$26,IF(W2&lt;=360,INFORME_MENSAL!$A$27,IF(W2&gt;360,INFORME_MENSAL!$A$28,)))))))),"")</f>
+        <f>IF(X2="Antecipação",IF(W2&lt;=30,INFORME_MENSAL!$A$21,IF(W2&lt;=60,INFORME_MENSAL!$A$22,IF(W2&lt;=90,INFORME_MENSAL!$A$23,IF(W2&lt;=120,INFORME_MENSAL!$A$24,IF(W2&lt;=150,INFORME_MENSAL!$A$25,IF(W2&lt;=180,INFORME_MENSAL!$A$26,IF(W2&lt;=360,INFORME_MENSAL!$A$27,IF(W2&gt;360,INFORME_MENSAL!$A$28)))))))),"")</f>
         <v/>
       </c>
     </row>
@@ -33413,7 +33366,7 @@
         <v/>
       </c>
       <c r="Z3">
-        <f>IF(X3="Antecipação",IF(W3&lt;=30,INFORME_MENSAL!$A$21,IF(W3&lt;=60,INFORME_MENSAL!$A$22,IF(W3&lt;=90,INFORME_MENSAL!$A$23,IF(W3&lt;=120,INFORME_MENSAL!$A$24,IF(W3&lt;=150,INFORME_MENSAL!$A$25,IF(W3&lt;=180,INFORME_MENSAL!$A$26,IF(W3&lt;=360,INFORME_MENSAL!$A$27,IF(W3&gt;360,INFORME_MENSAL!$A$28,)))))))),"")</f>
+        <f>IF(X3="Antecipação",IF(W3&lt;=30,INFORME_MENSAL!$A$21,IF(W3&lt;=60,INFORME_MENSAL!$A$22,IF(W3&lt;=90,INFORME_MENSAL!$A$23,IF(W3&lt;=120,INFORME_MENSAL!$A$24,IF(W3&lt;=150,INFORME_MENSAL!$A$25,IF(W3&lt;=180,INFORME_MENSAL!$A$26,IF(W3&lt;=360,INFORME_MENSAL!$A$27,IF(W3&gt;360,INFORME_MENSAL!$A$28)))))))),"")</f>
         <v/>
       </c>
     </row>
@@ -33505,7 +33458,7 @@
         <v/>
       </c>
       <c r="Z4">
-        <f>IF(X4="Antecipação",IF(W4&lt;=30,INFORME_MENSAL!$A$21,IF(W4&lt;=60,INFORME_MENSAL!$A$22,IF(W4&lt;=90,INFORME_MENSAL!$A$23,IF(W4&lt;=120,INFORME_MENSAL!$A$24,IF(W4&lt;=150,INFORME_MENSAL!$A$25,IF(W4&lt;=180,INFORME_MENSAL!$A$26,IF(W4&lt;=360,INFORME_MENSAL!$A$27,IF(W4&gt;360,INFORME_MENSAL!$A$28,)))))))),"")</f>
+        <f>IF(X4="Antecipação",IF(W4&lt;=30,INFORME_MENSAL!$A$21,IF(W4&lt;=60,INFORME_MENSAL!$A$22,IF(W4&lt;=90,INFORME_MENSAL!$A$23,IF(W4&lt;=120,INFORME_MENSAL!$A$24,IF(W4&lt;=150,INFORME_MENSAL!$A$25,IF(W4&lt;=180,INFORME_MENSAL!$A$26,IF(W4&lt;=360,INFORME_MENSAL!$A$27,IF(W4&gt;360,INFORME_MENSAL!$A$28)))))))),"")</f>
         <v/>
       </c>
     </row>
@@ -33597,7 +33550,7 @@
         <v/>
       </c>
       <c r="Z5">
-        <f>IF(X5="Antecipação",IF(W5&lt;=30,INFORME_MENSAL!$A$21,IF(W5&lt;=60,INFORME_MENSAL!$A$22,IF(W5&lt;=90,INFORME_MENSAL!$A$23,IF(W5&lt;=120,INFORME_MENSAL!$A$24,IF(W5&lt;=150,INFORME_MENSAL!$A$25,IF(W5&lt;=180,INFORME_MENSAL!$A$26,IF(W5&lt;=360,INFORME_MENSAL!$A$27,IF(W5&gt;360,INFORME_MENSAL!$A$28,)))))))),"")</f>
+        <f>IF(X5="Antecipação",IF(W5&lt;=30,INFORME_MENSAL!$A$21,IF(W5&lt;=60,INFORME_MENSAL!$A$22,IF(W5&lt;=90,INFORME_MENSAL!$A$23,IF(W5&lt;=120,INFORME_MENSAL!$A$24,IF(W5&lt;=150,INFORME_MENSAL!$A$25,IF(W5&lt;=180,INFORME_MENSAL!$A$26,IF(W5&lt;=360,INFORME_MENSAL!$A$27,IF(W5&gt;360,INFORME_MENSAL!$A$28)))))))),"")</f>
         <v/>
       </c>
     </row>
@@ -33712,7 +33665,7 @@
   </sheetPr>
   <dimension ref="A1:S366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>

</xml_diff>